<commit_message>
Load 3: Load TA File + ML (Line Regression)
</commit_message>
<xml_diff>
--- a/data/interim/4_Traiding_Repotr_1.xlsx
+++ b/data/interim/4_Traiding_Repotr_1.xlsx
@@ -889,31 +889,31 @@
         <v>43830</v>
       </c>
       <c r="B18" t="n">
-        <v>10.49141302499574</v>
+        <v>22.83625233803775</v>
       </c>
       <c r="C18" t="n">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="D18" t="n">
-        <v>70.58823529411765</v>
+        <v>73.17073170731707</v>
       </c>
       <c r="E18" t="n">
-        <v>537.7508000000015</v>
+        <v>-1099.879599999999</v>
       </c>
       <c r="F18" t="n">
-        <v>1.175084133058028</v>
+        <v>-2.40343866756536</v>
       </c>
       <c r="G18" t="n">
-        <v>381384.0239499991</v>
+        <v>380289.5273999991</v>
       </c>
       <c r="H18" t="n">
-        <v>833.3940463602577</v>
+        <v>831.0023706443095</v>
       </c>
       <c r="I18" t="n">
-        <v>26.87352819155826</v>
+        <v>34.0305737928054</v>
       </c>
       <c r="J18" t="n">
-        <v>25</v>
+        <v>-20.73170731707317</v>
       </c>
       <c r="K18" t="n">
         <v>45762.74879999986</v>

</xml_diff>